<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@09dfc0b6299e9abfa74e5c9ae499f817effffc48 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-ymf262-bom.xlsx
+++ b/BoM/Costs/rcbus-ymf262-bom.xlsx
@@ -279,7 +279,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>C1 C3 C6 C7 C12</t>
+    <t>C1 C3 C6 C7 C12 C19</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -501,19 +501,19 @@
     <t>23</t>
   </si>
   <si>
-    <t>CXO_DIP-8-14</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>14.318MHz</t>
-  </si>
-  <si>
-    <t>Oscillator_DIP-8-14</t>
-  </si>
-  <si>
-    <t>http://cdn-reichelt.de/documents/datenblatt/B400/OSZI.pdf</t>
+    <t>ASV-xxxMHz</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>SG-8002CA</t>
+  </si>
+  <si>
+    <t>Oscillator_SMD_Abracon_ASV-4Pin_7.0x5.1mm</t>
+  </si>
+  <si>
+    <t>http://www.abracon.com/Oscillators/ASV.pdf</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -555,7 +555,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>39 (35 SMD/ 4 THT)</t>
+    <t>40 (37 SMD/ 3 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -618,7 +618,7 @@
     <t>Quad Low-Noise JFET-Input Operational Amplifiers, DIP-14/SOIC-14</t>
   </si>
   <si>
-    <t>Crystal Clock Oscillator, DIP8-style metal package</t>
+    <t>3.3V HCMOS SMD Crystal Clock Oscillator, Abracon</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -633,7 +633,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-08-21 22:40:17</t>
+    <t>2025-08-26 22:51:14</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -1084,8 +1084,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>83259</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>997659</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1423,12 +1423,12 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="9" max="9" width="52.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="30.7109375" customWidth="1"/>
@@ -1523,7 +1523,7 @@
         <v>132</v>
       </c>
       <c r="F6" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1846,7 +1846,7 @@
         <v>21</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>22</v>
@@ -2749,12 +2749,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="44.7109375" customWidth="1" outlineLevel="2"/>
     <col min="5" max="5" width="13.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="58.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="48.7109375" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
@@ -2996,8 +2996,8 @@
         <v>21</v>
       </c>
       <c r="G15" s="18">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="I15" s="19">
         <f>IF(AND(ISNUMBER(G15),ISNUMBER(H15)),G15*H15,"")</f>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@b43f424ddd5021915e267e75a2a8900653243e1b 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-ymf262-bom.xlsx
+++ b/BoM/Costs/rcbus-ymf262-bom.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="169">
   <si>
     <t>Row</t>
   </si>
@@ -291,10 +291,10 @@
     <t>C_Polarized_Small</t>
   </si>
   <si>
-    <t>C15 C16</t>
-  </si>
-  <si>
-    <t>10uf</t>
+    <t>C8 C15 C16</t>
+  </si>
+  <si>
+    <t>10uF</t>
   </si>
   <si>
     <t>8</t>
@@ -303,204 +303,195 @@
     <t>C4 C5</t>
   </si>
   <si>
-    <t>10uF</t>
-  </si>
-  <si>
     <t>C_1206_3216Metric</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>C8</t>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>SJ1-3523N</t>
+  </si>
+  <si>
+    <t>Headphone_Jack_3.5mm_5_pin</t>
+  </si>
+  <si>
+    <t>CP1-3523N-ND</t>
+  </si>
+  <si>
+    <t>Connectors, Interconnects</t>
+  </si>
+  <si>
+    <t>Barrel - Audio Connectors</t>
+  </si>
+  <si>
+    <t>https://www.cui.com/product/resource/digikeypdf/sj1-352xn_series.pdf</t>
+  </si>
+  <si>
+    <t>/product-detail/en/cui-inc/SJ1-3523N/CP1-3523N-ND/738689</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>CON1</t>
-  </si>
-  <si>
-    <t>SJ1-3523N</t>
-  </si>
-  <si>
-    <t>Headphone_Jack_3.5mm_5_pin</t>
-  </si>
-  <si>
-    <t>CP1-3523N-ND</t>
-  </si>
-  <si>
-    <t>Connectors, Interconnects</t>
-  </si>
-  <si>
-    <t>Barrel - Audio Connectors</t>
-  </si>
-  <si>
-    <t>https://www.cui.com/product/resource/digikeypdf/sj1-352xn_series.pdf</t>
-  </si>
-  <si>
-    <t>/product-detail/en/cui-inc/SJ1-3523N/CP1-3523N-ND/738689</t>
+    <t>Conn_02x06_Odd_Even</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>BASE ADDRESS</t>
+  </si>
+  <si>
+    <t>PinHeader_2x06_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>Conn_02x06_Odd_Even</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>BASE ADDRESS</t>
-  </si>
-  <si>
-    <t>PinHeader_2x06_P2.54mm_Vertical</t>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>33uH</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>33uH</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>BLM18PG221SN1D</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>BLM18PG221SN1D</t>
+    <t>Conn_01x39</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>RC2014 BUS</t>
+  </si>
+  <si>
+    <t>PinHeader_1x39_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>Conn_01x39</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>RC2014 BUS</t>
-  </si>
-  <si>
-    <t>PinHeader_1x39_P2.54mm_Vertical</t>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
+    <t>R10 R11</t>
+  </si>
+  <si>
+    <t>1K</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>R10 R11</t>
-  </si>
-  <si>
-    <t>1K</t>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R1 R2 R3 R4 R5 R6</t>
+  </si>
+  <si>
+    <t>10K</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R1 R2 R3 R4 R5 R6</t>
-  </si>
-  <si>
-    <t>10K</t>
+    <t>R8 R9</t>
+  </si>
+  <si>
+    <t>15k</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>R8 R9</t>
-  </si>
-  <si>
-    <t>15k</t>
+    <t>74HCT688</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>74HCT688</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
+    <t>TL074</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>TL074</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
+    <t>YAC512</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>YAC512</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
+    <t>YMF262</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SOP-24_7.5x15.4mm_P1.27mm</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>YMF262</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SOP-24_7.5x15.4mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>ASV-xxxMHz</t>
   </si>
   <si>
@@ -633,7 +624,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-08-26 22:51:14</t>
+    <t>2025-08-28 08:18:27</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -799,7 +790,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -845,12 +836,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF0BD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,7 +906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -989,17 +974,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1411,7 +1393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1440,7 +1422,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1458,55 +1440,55 @@
     </row>
     <row r="2" spans="1:16">
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F2" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="C4" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="C5" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1514,13 +1496,13 @@
     </row>
     <row r="6" spans="1:16">
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F6" s="3">
         <v>40</v>
@@ -1896,7 +1878,7 @@
         <v>21</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>22</v>
@@ -1940,10 +1922,10 @@
         <v>44</v>
       </c>
       <c r="E16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>24</v>
@@ -1976,24 +1958,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>16</v>
@@ -2004,46 +1986,46 @@
       <c r="I17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>17</v>
+      <c r="J17" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>17</v>
+      <c r="L17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="30" customHeight="1">
+    <row r="18" spans="1:16">
       <c r="A18" s="8" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>16</v>
@@ -2054,23 +2036,23 @@
       <c r="I18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="11" t="s">
-        <v>54</v>
+      <c r="J18" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="N18" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="O18" s="11" t="s">
-        <v>58</v>
+      <c r="L18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>17</v>
@@ -2078,22 +2060,22 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>16</v>
@@ -2128,22 +2110,22 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>16</v>
@@ -2184,16 +2166,16 @@
         <v>17</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>16</v>
@@ -2228,22 +2210,22 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>16</v>
@@ -2278,25 +2260,25 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>22</v>
@@ -2334,19 +2316,19 @@
         <v>17</v>
       </c>
       <c r="C24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>81</v>
-      </c>
       <c r="G24" s="8" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>22</v>
@@ -2378,13 +2360,13 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>87</v>
@@ -2393,10 +2375,10 @@
         <v>88</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>22</v>
@@ -2434,25 +2416,25 @@
         <v>17</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="F26" s="10" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>23</v>
+      <c r="I26" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="J26" s="9" t="s">
         <v>17</v>
@@ -2478,22 +2460,22 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>16</v>
@@ -2502,7 +2484,7 @@
         <v>22</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>17</v>
@@ -2528,22 +2510,22 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>16</v>
@@ -2551,8 +2533,8 @@
       <c r="H28" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="10" t="s">
-        <v>101</v>
+      <c r="I28" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>17</v>
@@ -2578,22 +2560,22 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>16</v>
@@ -2628,22 +2610,22 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>16</v>
@@ -2651,8 +2633,8 @@
       <c r="H30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>17</v>
+      <c r="I30" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="J30" s="9" t="s">
         <v>17</v>
@@ -2673,56 +2655,6 @@
         <v>17</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P31" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2738,7 +2670,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="9" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
@@ -2762,7 +2694,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2772,13 +2704,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="D2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I2" s="12">
         <v>1</v>
@@ -2786,13 +2718,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="D3" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I3" s="14">
         <f>TotalCost/BoardQty</f>
@@ -2801,38 +2733,38 @@
     </row>
     <row r="4" spans="1:9">
       <c r="D4" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I4" s="15">
-        <f>SUM(I10:I32)</f>
+        <f>SUM(I10:I31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="D5" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2857,19 +2789,19 @@
         <v>5</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="I9" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2880,7 +2812,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>21</v>
@@ -2902,7 +2834,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>21</v>
@@ -2924,7 +2856,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>21</v>
@@ -2946,7 +2878,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>21</v>
@@ -2968,7 +2900,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>21</v>
@@ -2990,7 +2922,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>21</v>
@@ -3012,14 +2944,14 @@
         <v>42</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="I16" s="19">
         <f>IF(AND(ISNUMBER(G16),ISNUMBER(H16)),G16*H16,"")</f>
@@ -3031,13 +2963,13 @@
         <v>44</v>
       </c>
       <c r="B17" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="G17" s="18">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3048,18 +2980,24 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="30" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C18" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>21</v>
+      <c r="F18" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="G18" s="18">
         <f>BoardQty*1</f>
@@ -3070,24 +3008,18 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1">
+    <row r="19" spans="1:9" ht="45" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G19" s="18">
         <f>BoardQty*1</f>
@@ -3098,18 +3030,18 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" customHeight="1">
+    <row r="20" spans="1:9">
       <c r="A20" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G20" s="18">
         <f>BoardQty*1</f>
@@ -3122,16 +3054,16 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G21" s="18">
         <f>BoardQty*1</f>
@@ -3142,18 +3074,18 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="30" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G22" s="18">
         <f>BoardQty*1</f>
@@ -3164,18 +3096,18 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1">
+    <row r="23" spans="1:9">
       <c r="A23" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G23" s="18">
         <f>BoardQty*1</f>
@@ -3188,20 +3120,20 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G24" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="I24" s="19">
         <f>IF(AND(ISNUMBER(G24),ISNUMBER(H24)),G24*H24,"")</f>
@@ -3210,20 +3142,20 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G25" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="I25" s="19">
         <f>IF(AND(ISNUMBER(G25),ISNUMBER(H25)),G25*H25,"")</f>
@@ -3238,14 +3170,14 @@
         <v>88</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G26" s="18">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="I26" s="19">
         <f>IF(AND(ISNUMBER(G26),ISNUMBER(H26)),G26*H26,"")</f>
@@ -3254,41 +3186,44 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="C27" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>81</v>
+        <v>92</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="G27" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="I27" s="19">
         <f>IF(AND(ISNUMBER(G27),ISNUMBER(H27)),G27*H27,"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="30" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G28" s="18">
         <f>BoardQty*1</f>
@@ -3299,21 +3234,15 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1">
+    <row r="29" spans="1:9">
       <c r="A29" s="18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G29" s="18">
         <f>BoardQty*1</f>
@@ -3326,13 +3255,13 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>103</v>
-      </c>
       <c r="D30" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G30" s="18">
         <f>BoardQty*1</f>
@@ -3345,13 +3274,19 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="G31" s="18">
         <f>BoardQty*1</f>
@@ -3362,42 +3297,17 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="G32" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="I32" s="19">
-        <f>IF(AND(ISNUMBER(G32),ISNUMBER(H32)),G32*H32,"")</f>
-        <v/>
+    <row r="34" spans="1:2">
+      <c r="A34" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="22" t="s">
-        <v>156</v>
+      <c r="A35" s="22" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3515,15 +3425,10 @@
       <formula>AND(ISBLANK(F31),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="expression" dxfId="0" priority="23">
-      <formula>AND(ISBLANK(F32),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F28" r:id="rId1"/>
-    <hyperlink ref="F29" r:id="rId2"/>
-    <hyperlink ref="F32" r:id="rId3"/>
+    <hyperlink ref="F27" r:id="rId1"/>
+    <hyperlink ref="F28" r:id="rId2"/>
+    <hyperlink ref="F31" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId4"/>
@@ -3544,77 +3449,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="23" t="s">
-        <v>160</v>
+      <c r="A4" s="11" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="24" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="26" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="25" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" s="27" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="26" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" s="28" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="27" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" s="29" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="28" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" s="30" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="29" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" s="31" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="30" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="32" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@ffcfb9396d06d84fb116886ae824cff65907a9a5 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-ymf262-bom.xlsx
+++ b/BoM/Costs/rcbus-ymf262-bom.xlsx
@@ -525,13 +525,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>@version@</t>
+    <t>0.0.1</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>@date@</t>
+    <t>${DATE}</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -624,7 +624,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-08-28 08:18:27</t>
+    <t>2025-08-28 22:24:02</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@291c25c960d7e0f6c5c821497c85d57fa4939298 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-ymf262-bom.xlsx
+++ b/BoM/Costs/rcbus-ymf262-bom.xlsx
@@ -624,7 +624,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-08-28 22:24:02</t>
+    <t>2025-08-31 09:06:19</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -2944,7 +2944,7 @@
         <v>42</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@9c8d0cd003b39a240463bae4e94c496cca633260 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-ymf262-bom.xlsx
+++ b/BoM/Costs/rcbus-ymf262-bom.xlsx
@@ -531,7 +531,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-09-02</t>
+    <t>2025-09-03</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -624,7 +624,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-09-02 22:48:47</t>
+    <t>2025-09-03 23:01:40</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@646990f17bd25725641340863379bc60f4c51cf2 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-ymf262-bom.xlsx
+++ b/BoM/Costs/rcbus-ymf262-bom.xlsx
@@ -531,7 +531,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-09-03</t>
+    <t>2025-09-11</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -624,7 +624,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-09-03 23:01:40</t>
+    <t>2025-09-11 23:27:30</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>